<commit_message>
swapped bonferroni-correction with fdr-correction and added descriptive stats about within-person variance in valence and arousal ratings
</commit_message>
<xml_diff>
--- a/Free-Mouse_Analysis/Results_Free-Mouse/Mixed-Model_Analysis/Result_Tables/Free_Pred_Coeffs_resTable.xlsx
+++ b/Free-Mouse_Analysis/Results_Free-Mouse/Mixed-Model_Analysis/Result_Tables/Free_Pred_Coeffs_resTable.xlsx
@@ -542,7 +542,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>targt</t>
+          <t>target</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
@@ -1774,7 +1774,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1791,7 +1791,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2252,7 +2252,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2824,7 +2824,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
@@ -3204,7 +3204,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
@@ -3298,7 +3298,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -3315,7 +3315,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
@@ -4834,7 +4834,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -4851,7 +4851,7 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">
@@ -5008,7 +5008,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>targt</t>
+          <t>target</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
@@ -6240,7 +6240,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -6257,7 +6257,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -6718,7 +6718,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -6735,7 +6735,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -8772,7 +8772,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -8866,7 +8866,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -8960,7 +8960,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -9300,7 +9300,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -9317,7 +9317,7 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>&lt; .05</t>
+          <t>&lt; .05*</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">

</xml_diff>